<commit_message>
lots of code update
cleaning it up a little. fixed SedFlux plto
</commit_message>
<xml_diff>
--- a/Data/Q/DAM_StormIntervals.xlsx
+++ b/Data/Q/DAM_StormIntervals.xlsx
@@ -20,16 +20,16 @@
     <t>next storm start</t>
   </si>
   <si>
-    <t>start</t>
-  </si>
-  <si>
-    <t>duration (min)</t>
+    <t>duration (hrs)</t>
   </si>
   <si>
     <t>end</t>
   </si>
   <si>
     <t>next storm end</t>
+  </si>
+  <si>
+    <t>start</t>
   </si>
 </sst>
 </file>
@@ -411,19 +411,19 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c s="1" r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c s="1" r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c s="1" r="D1" t="s">
         <v>1</v>
-      </c>
-      <c s="1" r="C1" t="s">
-        <v>3</v>
-      </c>
-      <c s="1" r="D1" t="s">
-        <v>2</v>
       </c>
       <c s="1" r="E1" t="s">
         <v>0</v>
       </c>
       <c s="1" r="F1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -437,7 +437,7 @@
         <v>40927.322916666664</v>
       </c>
       <c r="D2" t="n">
-        <v>26100000000000</v>
+        <v>7.25</v>
       </c>
       <c s="2" r="E2" t="n">
         <v>40927.5625</v>
@@ -457,7 +457,7 @@
         <v>40927.9375</v>
       </c>
       <c r="D3" t="n">
-        <v>32400000000000</v>
+        <v>9.0</v>
       </c>
       <c s="2" r="E3" t="n">
         <v>40933.15625</v>
@@ -477,7 +477,7 @@
         <v>40933.65625</v>
       </c>
       <c r="D4" t="n">
-        <v>43200000000000</v>
+        <v>12.0</v>
       </c>
       <c s="2" r="E4" t="n">
         <v>40941.25</v>
@@ -497,7 +497,7 @@
         <v>40941.75</v>
       </c>
       <c r="D5" t="n">
-        <v>43200000000000</v>
+        <v>12.0</v>
       </c>
       <c s="2" r="E5" t="n">
         <v>40942.052083333336</v>
@@ -517,7 +517,7 @@
         <v>40942.125</v>
       </c>
       <c r="D6" t="n">
-        <v>6300000000000</v>
+        <v>1.75</v>
       </c>
       <c s="2" r="E6" t="n">
         <v>40942.135416666664</v>
@@ -537,7 +537,7 @@
         <v>40942.21875</v>
       </c>
       <c r="D7" t="n">
-        <v>7200000000000</v>
+        <v>2.0</v>
       </c>
       <c s="2" r="E7" t="n">
         <v>40942.322916666664</v>
@@ -557,7 +557,7 @@
         <v>40942.895833333336</v>
       </c>
       <c r="D8" t="n">
-        <v>49500000000000</v>
+        <v>13.75</v>
       </c>
       <c s="2" r="E8" t="n">
         <v>40944.416666666664</v>
@@ -577,7 +577,7 @@
         <v>40944.895833333336</v>
       </c>
       <c r="D9" t="n">
-        <v>41400000000000</v>
+        <v>11.5</v>
       </c>
       <c s="2" r="E9" t="n">
         <v>40944.958333333336</v>
@@ -597,7 +597,7 @@
         <v>40946.8125</v>
       </c>
       <c r="D10" t="n">
-        <v>146700000000000</v>
+        <v>40.75</v>
       </c>
       <c s="2" r="E10" t="n">
         <v>40946.65625</v>
@@ -617,7 +617,7 @@
         <v>40963.21875</v>
       </c>
       <c r="D11" t="n">
-        <v>29700000000000</v>
+        <v>8.25</v>
       </c>
       <c s="2" r="E11" t="n">
         <v>40977.25</v>
@@ -637,7 +637,7 @@
         <v>40977.479166666664</v>
       </c>
       <c r="D12" t="n">
-        <v>19800000000000</v>
+        <v>5.5</v>
       </c>
       <c s="2" r="E12" t="n">
         <v>40984.520833333336</v>
@@ -657,7 +657,7 @@
         <v>40984.677083333336</v>
       </c>
       <c r="D13" t="n">
-        <v>13500000000000</v>
+        <v>3.75</v>
       </c>
       <c s="2" r="E13" t="n">
         <v>40985.489583333336</v>
@@ -677,7 +677,7 @@
         <v>40985.739583333336</v>
       </c>
       <c r="D14" t="n">
-        <v>21600000000000</v>
+        <v>6.0</v>
       </c>
       <c s="2" r="E14" t="n">
         <v>40989.84375</v>
@@ -697,7 +697,7 @@
         <v>40990.145833333336</v>
       </c>
       <c r="D15" t="n">
-        <v>26100000000000</v>
+        <v>7.25</v>
       </c>
       <c s="2" r="E15" t="n">
         <v>40990.21875</v>
@@ -717,7 +717,7 @@
         <v>40990.302083333336</v>
       </c>
       <c r="D16" t="n">
-        <v>7200000000000</v>
+        <v>2.0</v>
       </c>
       <c s="2" r="E16" t="n">
         <v>40990.90625</v>
@@ -737,7 +737,7 @@
         <v>40991.322916666664</v>
       </c>
       <c r="D17" t="n">
-        <v>36000000000000</v>
+        <v>10.0</v>
       </c>
       <c s="2" r="E17" t="n">
         <v>40993.145833333336</v>
@@ -757,7 +757,7 @@
         <v>40993.9375</v>
       </c>
       <c r="D18" t="n">
-        <v>68400000000000</v>
+        <v>19.0</v>
       </c>
       <c s="2" r="E18" t="n">
         <v>41037.197916666664</v>
@@ -777,7 +777,7 @@
         <v>41037.322916666664</v>
       </c>
       <c r="D19" t="n">
-        <v>10800000000000</v>
+        <v>3.0</v>
       </c>
       <c s="2" r="E19" t="n">
         <v>41051.78125</v>
@@ -797,7 +797,7 @@
         <v>41052.125</v>
       </c>
       <c r="D20" t="n">
-        <v>29700000000000</v>
+        <v>8.25</v>
       </c>
       <c s="2" r="E20" t="n">
         <v>41052.322916666664</v>
@@ -817,7 +817,7 @@
         <v>41053.5625</v>
       </c>
       <c r="D21" t="n">
-        <v>107100000000000</v>
+        <v>29.75</v>
       </c>
       <c s="2" r="E21" t="n">
         <v>41053.833333333336</v>
@@ -837,7 +837,7 @@
         <v>41054.708333333336</v>
       </c>
       <c r="D22" t="n">
-        <v>75600000000000</v>
+        <v>21.0</v>
       </c>
       <c s="2" r="E22" t="n">
         <v>41055.0625</v>
@@ -857,7 +857,7 @@
         <v>41055.697916666664</v>
       </c>
       <c r="D23" t="n">
-        <v>54900000000000</v>
+        <v>15.25</v>
       </c>
       <c s="2" r="E23" t="n">
         <v>41063.427083333336</v>
@@ -877,7 +877,7 @@
         <v>41063.885416666664</v>
       </c>
       <c r="D24" t="n">
-        <v>39600000000000</v>
+        <v>11.0</v>
       </c>
       <c s="2" r="E24" t="n">
         <v>41064.010416666664</v>
@@ -897,7 +897,7 @@
         <v>41064.46875</v>
       </c>
       <c r="D25" t="n">
-        <v>39600000000000</v>
+        <v>11.0</v>
       </c>
       <c s="2" r="E25" t="n">
         <v>41064.604166666664</v>
@@ -917,7 +917,7 @@
         <v>41065.875</v>
       </c>
       <c r="D26" t="n">
-        <v>109800000000000</v>
+        <v>30.5</v>
       </c>
       <c s="2" r="E26" t="n">
         <v>41066.885416666664</v>
@@ -937,7 +937,7 @@
         <v>41067.15625</v>
       </c>
       <c r="D27" t="n">
-        <v>23400000000000</v>
+        <v>6.5</v>
       </c>
       <c s="2" r="E27" t="n">
         <v>41067.322916666664</v>
@@ -957,7 +957,7 @@
         <v>41067.729166666664</v>
       </c>
       <c r="D28" t="n">
-        <v>35100000000000</v>
+        <v>9.75</v>
       </c>
       <c s="2" r="E28" t="n">
         <v>41098.083333333336</v>
@@ -977,7 +977,7 @@
         <v>41098.25</v>
       </c>
       <c r="D29" t="n">
-        <v>14400000000000</v>
+        <v>4.0</v>
       </c>
       <c s="2" r="E29" t="n">
         <v>41130.145833333336</v>
@@ -997,7 +997,7 @@
         <v>41130.364583333336</v>
       </c>
       <c r="D30" t="n">
-        <v>18900000000000</v>
+        <v>5.25</v>
       </c>
       <c s="2" r="E30" t="n">
         <v>41153.479166666664</v>
@@ -1017,7 +1017,7 @@
         <v>41153.78125</v>
       </c>
       <c r="D31" t="n">
-        <v>26100000000000</v>
+        <v>7.25</v>
       </c>
       <c s="2" r="E31" t="n">
         <v>41153.791666666664</v>
@@ -1037,7 +1037,7 @@
         <v>41155.135416666664</v>
       </c>
       <c r="D32" t="n">
-        <v>116100000000000</v>
+        <v>32.25</v>
       </c>
       <c s="2" r="E32" t="n">
         <v>41316.864583333336</v>
@@ -1057,7 +1057,7 @@
         <v>41317.53125</v>
       </c>
       <c r="D33" t="n">
-        <v>57600000000000</v>
+        <v>16.0</v>
       </c>
       <c s="2" r="E33" t="n">
         <v>41338.770833333336</v>
@@ -1077,7 +1077,7 @@
         <v>41339.09375</v>
       </c>
       <c r="D34" t="n">
-        <v>27900000000000</v>
+        <v>7.75</v>
       </c>
       <c s="2" r="E34" t="n">
         <v>41339.375</v>
@@ -1097,7 +1097,7 @@
         <v>41339.947916666664</v>
       </c>
       <c r="D35" t="n">
-        <v>49500000000000</v>
+        <v>13.75</v>
       </c>
       <c s="2" r="E35" t="n">
         <v>41340.583333333336</v>
@@ -1117,7 +1117,7 @@
         <v>41341.916666666664</v>
       </c>
       <c r="D36" t="n">
-        <v>115200000000000</v>
+        <v>32.0</v>
       </c>
       <c s="2" r="E36" t="n">
         <v>41344.083333333336</v>
@@ -1137,7 +1137,7 @@
         <v>41344.833333333336</v>
       </c>
       <c r="D37" t="n">
-        <v>64800000000000</v>
+        <v>18.0</v>
       </c>
       <c s="2" r="E37" t="n">
         <v>41354.541666666664</v>
@@ -1157,7 +1157,7 @@
         <v>41354.635416666664</v>
       </c>
       <c r="D38" t="n">
-        <v>8100000000000</v>
+        <v>2.25</v>
       </c>
       <c s="2" r="E38" t="n">
         <v>41356.447916666664</v>
@@ -1177,7 +1177,7 @@
         <v>41356.520833333336</v>
       </c>
       <c r="D39" t="n">
-        <v>6300000000000</v>
+        <v>1.75</v>
       </c>
       <c s="2" r="E39" t="n">
         <v>41380.447916666664</v>
@@ -1197,7 +1197,7 @@
         <v>41381.947916666664</v>
       </c>
       <c r="D40" t="n">
-        <v>129600000000000</v>
+        <v>36.0</v>
       </c>
       <c s="2" r="E40" t="n">
         <v>41382.625</v>
@@ -1217,7 +1217,7 @@
         <v>41382.697916666664</v>
       </c>
       <c r="D41" t="n">
-        <v>6300000000000</v>
+        <v>1.75</v>
       </c>
       <c s="2" r="E41" t="n">
         <v>41382.791666666664</v>
@@ -1237,7 +1237,7 @@
         <v>41382.979166666664</v>
       </c>
       <c r="D42" t="n">
-        <v>16200000000000</v>
+        <v>4.5</v>
       </c>
       <c s="2" r="E42" t="n">
         <v>41384.15625</v>
@@ -1257,7 +1257,7 @@
         <v>41384.9375</v>
       </c>
       <c r="D43" t="n">
-        <v>67500000000000</v>
+        <v>18.75</v>
       </c>
       <c s="2" r="E43" t="n">
         <v>41387.541666666664</v>
@@ -1277,7 +1277,7 @@
         <v>41388.947916666664</v>
       </c>
       <c r="D44" t="n">
-        <v>121500000000000</v>
+        <v>33.75</v>
       </c>
       <c s="2" r="E44" t="n">
         <v>41392.083333333336</v>
@@ -1297,7 +1297,7 @@
         <v>41392.177083333336</v>
       </c>
       <c r="D45" t="n">
-        <v>8100000000000</v>
+        <v>2.25</v>
       </c>
       <c s="2" r="E45" t="n">
         <v>41392.40625</v>
@@ -1317,7 +1317,7 @@
         <v>41393.822916666664</v>
       </c>
       <c r="D46" t="n">
-        <v>122400000000000</v>
+        <v>34.0</v>
       </c>
       <c s="2" r="E46" t="n">
         <v>41394.59375</v>
@@ -1337,7 +1337,7 @@
         <v>41396.15625</v>
       </c>
       <c r="D47" t="n">
-        <v>135000000000000</v>
+        <v>37.5</v>
       </c>
       <c s="2" r="E47" t="n">
         <v>41405.59375</v>
@@ -1357,7 +1357,7 @@
         <v>41405.833333333336</v>
       </c>
       <c r="D48" t="n">
-        <v>20700000000000</v>
+        <v>5.75</v>
       </c>
       <c s="2" r="E48" t="n">
         <v>41430.135416666664</v>
@@ -1377,7 +1377,7 @@
         <v>41431.854166666664</v>
       </c>
       <c r="D49" t="n">
-        <v>148500000000000</v>
+        <v>41.25</v>
       </c>
       <c s="2" r="E49" t="n">
         <v>41441.114583333336</v>
@@ -1397,7 +1397,7 @@
         <v>41441.729166666664</v>
       </c>
       <c r="D50" t="n">
-        <v>53100000000000</v>
+        <v>14.75</v>
       </c>
       <c s="2" r="E50" t="n">
         <v>41468.708333333336</v>
@@ -1417,7 +1417,7 @@
         <v>41468.833333333336</v>
       </c>
       <c r="D51" t="n">
-        <v>10800000000000</v>
+        <v>3.0</v>
       </c>
       <c s="2" r="E51" t="n">
         <v>41472.135416666664</v>
@@ -1437,7 +1437,7 @@
         <v>41472.322916666664</v>
       </c>
       <c r="D52" t="n">
-        <v>16200000000000</v>
+        <v>4.5</v>
       </c>
       <c s="2" r="E52" t="n">
         <v>41472.947916666664</v>
@@ -1457,7 +1457,7 @@
         <v>41473.729166666664</v>
       </c>
       <c r="D53" t="n">
-        <v>67500000000000</v>
+        <v>18.75</v>
       </c>
       <c s="2" r="E53" t="n">
         <v>41474.0625</v>
@@ -1477,7 +1477,7 @@
         <v>41475.9375</v>
       </c>
       <c r="D54" t="n">
-        <v>162000000000000</v>
+        <v>45.0</v>
       </c>
       <c s="2" r="E54" t="n">
         <v>41482.9375</v>
@@ -1497,7 +1497,7 @@
         <v>41483.135416666664</v>
       </c>
       <c r="D55" t="n">
-        <v>17100000000000</v>
+        <v>4.75</v>
       </c>
       <c s="2" r="E55" t="n">
         <v>41489.666666666664</v>
@@ -1517,7 +1517,7 @@
         <v>41489.802083333336</v>
       </c>
       <c r="D56" t="n">
-        <v>11700000000000</v>
+        <v>3.25</v>
       </c>
       <c s="2" r="E56" t="n">
         <v>41491.9375</v>
@@ -1537,7 +1537,7 @@
         <v>41492.416666666664</v>
       </c>
       <c r="D57" t="n">
-        <v>41400000000000</v>
+        <v>11.5</v>
       </c>
       <c s="2" r="E57" t="n">
         <v>41496.177083333336</v>
@@ -1557,7 +1557,7 @@
         <v>41497.135416666664</v>
       </c>
       <c r="D58" t="n">
-        <v>82800000000000</v>
+        <v>23.0</v>
       </c>
       <c s="2" r="E58" t="n">
         <v>41501.78125</v>
@@ -1577,7 +1577,7 @@
         <v>41501.958333333336</v>
       </c>
       <c r="D59" t="n">
-        <v>15300000000000</v>
+        <v>4.25</v>
       </c>
       <c s="2" r="E59" t="n">
         <v>41502.322916666664</v>
@@ -1597,7 +1597,7 @@
         <v>41504.572916666664</v>
       </c>
       <c r="D60" t="n">
-        <v>194400000000000</v>
+        <v>54.0</v>
       </c>
       <c s="2" r="E60" t="n">
         <v>41505.270833333336</v>
@@ -1617,7 +1617,7 @@
         <v>41505.854166666664</v>
       </c>
       <c r="D61" t="n">
-        <v>50400000000000</v>
+        <v>14.0</v>
       </c>
       <c s="2" r="E61" t="n">
         <v>41518.1875</v>
@@ -1637,7 +1637,7 @@
         <v>41518.260416666664</v>
       </c>
       <c r="D62" t="n">
-        <v>6300000000000</v>
+        <v>1.75</v>
       </c>
       <c s="2" r="E62" t="n">
         <v>41518.34375</v>
@@ -1657,7 +1657,7 @@
         <v>41518.572916666664</v>
       </c>
       <c r="D63" t="n">
-        <v>19800000000000</v>
+        <v>5.5</v>
       </c>
       <c s="2" r="E63" t="n">
         <v>41684.625</v>
@@ -1677,7 +1677,7 @@
         <v>41684.8125</v>
       </c>
       <c r="D64" t="n">
-        <v>16200000000000</v>
+        <v>4.5</v>
       </c>
       <c s="2" r="E64" t="n">
         <v>41690.46875</v>
@@ -1697,7 +1697,7 @@
         <v>41690.75</v>
       </c>
       <c r="D65" t="n">
-        <v>24300000000000</v>
+        <v>6.75</v>
       </c>
       <c s="2" r="E65" t="n">
         <v>41691.479166666664</v>
@@ -1717,7 +1717,7 @@
         <v>41692.145833333336</v>
       </c>
       <c r="D66" t="n">
-        <v>57600000000000</v>
+        <v>16.0</v>
       </c>
       <c s="2" r="E66" t="n">
         <v>41695.885416666664</v>
@@ -1737,7 +1737,7 @@
         <v>41696.677083333336</v>
       </c>
       <c r="D67" t="n">
-        <v>68400000000000</v>
+        <v>19.0</v>
       </c>
       <c s="2" r="E67" t="n">
         <v>41697.083333333336</v>
@@ -1757,7 +1757,7 @@
         <v>41697.53125</v>
       </c>
       <c r="D68" t="n">
-        <v>38700000000000</v>
+        <v>10.75</v>
       </c>
       <c s="2" r="E68" t="n">
         <v>41697.677083333336</v>
@@ -1777,7 +1777,7 @@
         <v>41698.010416666664</v>
       </c>
       <c r="D69" t="n">
-        <v>28800000000000</v>
+        <v>8.0</v>
       </c>
       <c s="2" r="E69" t="n">
         <v>41704.822916666664</v>
@@ -1797,7 +1797,7 @@
         <v>41705.197916666664</v>
       </c>
       <c r="D70" t="n">
-        <v>32400000000000</v>
+        <v>9.0</v>
       </c>
       <c s="2" r="E70" t="n">
         <v>41711.520833333336</v>
@@ -1817,7 +1817,7 @@
         <v>41711.635416666664</v>
       </c>
       <c r="D71" t="n">
-        <v>9900000000000</v>
+        <v>2.75</v>
       </c>
       <c s="2" r="E71" t="n">
         <v>41711.666666666664</v>
@@ -1837,7 +1837,7 @@
         <v>41711.791666666664</v>
       </c>
       <c r="D72" t="n">
-        <v>10800000000000</v>
+        <v>3.0</v>
       </c>
       <c s="2" r="E72" t="n">
         <v>41711.833333333336</v>
@@ -1857,7 +1857,7 @@
         <v>41711.927083333336</v>
       </c>
       <c r="D73" t="n">
-        <v>8100000000000</v>
+        <v>2.25</v>
       </c>
       <c s="2" r="E73" t="n">
         <v>41712.020833333336</v>
@@ -1877,7 +1877,7 @@
         <v>41712.34375</v>
       </c>
       <c r="D74" t="n">
-        <v>27900000000000</v>
+        <v>7.75</v>
       </c>
       <c s="2" r="E74" t="n">
         <v>41735.520833333336</v>
@@ -1897,7 +1897,7 @@
         <v>41735.989583333336</v>
       </c>
       <c r="D75" t="n">
-        <v>40500000000000</v>
+        <v>11.25</v>
       </c>
       <c s="2" r="E75" t="n">
         <v>41737.604166666664</v>
@@ -1917,7 +1917,7 @@
         <v>41737.770833333336</v>
       </c>
       <c r="D76" t="n">
-        <v>14400000000000</v>
+        <v>4.0</v>
       </c>
       <c s="2" r="E76" t="n">
         <v>41738.989583333336</v>
@@ -1937,7 +1937,7 @@
         <v>41739.15625</v>
       </c>
       <c r="D77" t="n">
-        <v>14400000000000</v>
+        <v>4.0</v>
       </c>
       <c s="2" r="E77" t="n">
         <v>41747.791666666664</v>
@@ -1957,7 +1957,7 @@
         <v>41747.958333333336</v>
       </c>
       <c r="D78" t="n">
-        <v>14400000000000</v>
+        <v>4.0</v>
       </c>
       <c s="2" r="E78" t="n">
         <v>41748.291666666664</v>
@@ -1977,7 +1977,7 @@
         <v>41748.927083333336</v>
       </c>
       <c r="D79" t="n">
-        <v>54900000000000</v>
+        <v>15.25</v>
       </c>
       <c s="2" r="E79" t="n">
         <v>41748.958333333336</v>
@@ -1997,7 +1997,7 @@
         <v>41749.40625</v>
       </c>
       <c r="D80" t="n">
-        <v>38700000000000</v>
+        <v>10.75</v>
       </c>
       <c s="2" r="E80" t="n">
         <v>41754.65625</v>
@@ -2017,7 +2017,7 @@
         <v>41754.791666666664</v>
       </c>
       <c r="D81" t="n">
-        <v>11700000000000</v>
+        <v>3.25</v>
       </c>
       <c s="2" r="E81" t="n">
         <v>41756.489583333336</v>
@@ -2037,7 +2037,7 @@
         <v>41756.822916666664</v>
       </c>
       <c r="D82" t="n">
-        <v>28800000000000</v>
+        <v>8.0</v>
       </c>
       <c s="2" r="E82" t="n">
         <v>41757.385416666664</v>
@@ -2057,7 +2057,7 @@
         <v>41757.53125</v>
       </c>
       <c r="D83" t="n">
-        <v>12600000000000</v>
+        <v>3.5</v>
       </c>
       <c s="2" r="E83" t="n">
         <v>41757.885416666664</v>
@@ -2077,7 +2077,7 @@
         <v>41758.541666666664</v>
       </c>
       <c r="D84" t="n">
-        <v>56700000000000</v>
+        <v>15.75</v>
       </c>
       <c s="2" r="E84" t="n">
         <v>41759.489583333336</v>
@@ -2097,7 +2097,7 @@
         <v>41760.145833333336</v>
       </c>
       <c r="D85" t="n">
-        <v>56700000000000</v>
+        <v>15.75</v>
       </c>
       <c s="2" r="E85" t="n">
         <v>41778.5625</v>
@@ -2117,7 +2117,7 @@
         <v>41778.677083333336</v>
       </c>
       <c r="D86" t="n">
-        <v>9900000000000</v>
+        <v>2.75</v>
       </c>
       <c s="2" r="E86" t="n">
         <v>41779.041666666664</v>
@@ -2137,7 +2137,7 @@
         <v>41779.1875</v>
       </c>
       <c r="D87" t="n">
-        <v>12600000000000</v>
+        <v>3.5</v>
       </c>
       <c s="2" r="E87" t="n">
         <v>41781.5625</v>
@@ -2157,7 +2157,7 @@
         <v>41782.104166666664</v>
       </c>
       <c r="D88" t="n">
-        <v>46800000000000</v>
+        <v>13.0</v>
       </c>
       <c s="2" r="E88" t="n">
         <v>41795.802083333336</v>
@@ -2177,7 +2177,7 @@
         <v>41796.583333333336</v>
       </c>
       <c r="D89" t="n">
-        <v>67500000000000</v>
+        <v>18.75</v>
       </c>
       <c s="2" r="E89" t="n">
         <v>41807.072916666664</v>
@@ -2197,7 +2197,7 @@
         <v>41807.34375</v>
       </c>
       <c r="D90" t="n">
-        <v>23400000000000</v>
+        <v>6.5</v>
       </c>
       <c s="2" r="E90" t="n">
         <v>41823.4375</v>
@@ -2217,7 +2217,7 @@
         <v>41823.8125</v>
       </c>
       <c r="D91" t="n">
-        <v>32400000000000</v>
+        <v>9.0</v>
       </c>
       <c s="2" r="E91" t="n">
         <v>41825.25</v>
@@ -2237,7 +2237,7 @@
         <v>41825.71875</v>
       </c>
       <c r="D92" t="n">
-        <v>40500000000000</v>
+        <v>11.25</v>
       </c>
       <c s="2" r="E92" t="n">
         <v>41826.84375</v>
@@ -2257,7 +2257,7 @@
         <v>41826.96875</v>
       </c>
       <c r="D93" t="n">
-        <v>10800000000000</v>
+        <v>3.0</v>
       </c>
       <c s="2" r="E93" t="n">
         <v>41849.25</v>
@@ -2277,7 +2277,7 @@
         <v>41853.125</v>
       </c>
       <c r="D94" t="n">
-        <v>334800000000000</v>
+        <v>93.0</v>
       </c>
       <c s="2" r="E94" t="n">
         <v>41853.552083333336</v>
@@ -2297,7 +2297,7 @@
         <v>41854.510416666664</v>
       </c>
       <c r="D95" t="n">
-        <v>82800000000000</v>
+        <v>23.0</v>
       </c>
       <c s="2" r="E95" t="n">
         <v>41927.53125</v>
@@ -2317,7 +2317,7 @@
         <v>41927.697916666664</v>
       </c>
       <c r="D96" t="n">
-        <v>14400000000000</v>
+        <v>4.0</v>
       </c>
       <c s="2" r="E96" t="n">
         <v>41927.739583333336</v>
@@ -2337,7 +2337,7 @@
         <v>41928.114583333336</v>
       </c>
       <c r="D97" t="n">
-        <v>32400000000000</v>
+        <v>9.0</v>
       </c>
       <c s="2" r="E97" t="n">
         <v>41945.072916666664</v>
@@ -2357,7 +2357,7 @@
         <v>41945.385416666664</v>
       </c>
       <c r="D98" t="n">
-        <v>27000000000000</v>
+        <v>7.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Tried to fix everything
still not working
</commit_message>
<xml_diff>
--- a/Data/Q/DAM_StormIntervals.xlsx
+++ b/Data/Q/DAM_StormIntervals.xlsx
@@ -15,12 +15,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="5">
   <si>
-    <t>start</t>
+    <t>next storm start</t>
+  </si>
+  <si>
+    <t>duration (hrs)</t>
   </si>
   <si>
     <t>end</t>
+  </si>
+  <si>
+    <t>next storm end</t>
+  </si>
+  <si>
+    <t>start</t>
   </si>
 </sst>
 </file>
@@ -384,7 +393,7 @@
   <sheetPr>
     <outlinePr summaryRight="1" summaryBelow="1"/>
   </sheetPr>
-  <dimension ref="A1:C93"/>
+  <dimension ref="A1:F98"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1" activeCell="A1"/>
@@ -395,17 +404,29 @@
     <col max="1" collapsed="0" width="9.10" min="1"/>
     <col max="3" collapsed="0" width="9.10" min="3"/>
     <col max="2" collapsed="0" width="9.10" min="2"/>
+    <col max="5" collapsed="0" width="9.10" min="5"/>
+    <col max="4" collapsed="0" width="9.10" min="4"/>
+    <col max="6" collapsed="0" width="9.10" min="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:6">
       <c s="1" r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c s="1" r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c s="1" r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c s="1" r="E1" t="s">
         <v>0</v>
       </c>
-      <c s="1" r="C1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
+      <c s="1" r="F1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c s="1" r="A2" t="n">
         <v>0</v>
       </c>
@@ -415,8 +436,17 @@
       <c s="2" r="C2" t="n">
         <v>40927.322916666664</v>
       </c>
-    </row>
-    <row r="3" spans="1:3">
+      <c r="D2" t="n">
+        <v>7.25</v>
+      </c>
+      <c s="2" r="E2" t="n">
+        <v>40927.5625</v>
+      </c>
+      <c s="2" r="F2" t="n">
+        <v>40927.9375</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c s="1" r="A3" t="n">
         <v>1</v>
       </c>
@@ -426,995 +456,1908 @@
       <c s="2" r="C3" t="n">
         <v>40927.9375</v>
       </c>
-    </row>
-    <row r="4" spans="1:3">
+      <c r="D3" t="n">
+        <v>9.0</v>
+      </c>
+      <c s="2" r="E3" t="n">
+        <v>40933.15625</v>
+      </c>
+      <c s="2" r="F3" t="n">
+        <v>40933.65625</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c s="1" r="A4" t="n">
+        <v>2</v>
+      </c>
+      <c s="2" r="B4" t="n">
+        <v>40933.15625</v>
+      </c>
+      <c s="2" r="C4" t="n">
+        <v>40933.65625</v>
+      </c>
+      <c r="D4" t="n">
+        <v>12.0</v>
+      </c>
+      <c s="2" r="E4" t="n">
+        <v>40941.25</v>
+      </c>
+      <c s="2" r="F4" t="n">
+        <v>40941.75</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c s="1" r="A5" t="n">
         <v>3</v>
       </c>
-      <c s="2" r="B4" t="n">
+      <c s="2" r="B5" t="n">
         <v>40941.25</v>
       </c>
-      <c s="2" r="C4" t="n">
+      <c s="2" r="C5" t="n">
         <v>40941.75</v>
       </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c s="1" r="A5" t="n">
+      <c r="D5" t="n">
+        <v>12.0</v>
+      </c>
+      <c s="2" r="E5" t="n">
+        <v>40942.052083333336</v>
+      </c>
+      <c s="2" r="F5" t="n">
+        <v>40942.125</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c s="1" r="A6" t="n">
         <v>4</v>
       </c>
-      <c s="2" r="B5" t="n">
+      <c s="2" r="B6" t="n">
         <v>40942.052083333336</v>
       </c>
-      <c s="2" r="C5" t="n">
+      <c s="2" r="C6" t="n">
+        <v>40942.125</v>
+      </c>
+      <c r="D6" t="n">
+        <v>1.75</v>
+      </c>
+      <c s="2" r="E6" t="n">
+        <v>40942.135416666664</v>
+      </c>
+      <c s="2" r="F6" t="n">
         <v>40942.21875</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
-      <c s="1" r="A6" t="n">
+    <row r="7" spans="1:6">
+      <c s="1" r="A7" t="n">
+        <v>5</v>
+      </c>
+      <c s="2" r="B7" t="n">
+        <v>40942.135416666664</v>
+      </c>
+      <c s="2" r="C7" t="n">
+        <v>40942.21875</v>
+      </c>
+      <c r="D7" t="n">
+        <v>2.0</v>
+      </c>
+      <c s="2" r="E7" t="n">
+        <v>40942.322916666664</v>
+      </c>
+      <c s="2" r="F7" t="n">
+        <v>40942.895833333336</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c s="1" r="A8" t="n">
         <v>6</v>
       </c>
-      <c s="2" r="B6" t="n">
+      <c s="2" r="B8" t="n">
         <v>40942.322916666664</v>
       </c>
-      <c s="2" r="C6" t="n">
+      <c s="2" r="C8" t="n">
         <v>40942.895833333336</v>
       </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c s="1" r="A7" t="n">
+      <c r="D8" t="n">
+        <v>13.75</v>
+      </c>
+      <c s="2" r="E8" t="n">
+        <v>40944.416666666664</v>
+      </c>
+      <c s="2" r="F8" t="n">
+        <v>40944.895833333336</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c s="1" r="A9" t="n">
         <v>7</v>
       </c>
-      <c s="2" r="B7" t="n">
+      <c s="2" r="B9" t="n">
         <v>40944.416666666664</v>
       </c>
-      <c s="2" r="C7" t="n">
+      <c s="2" r="C9" t="n">
         <v>40944.895833333336</v>
       </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c s="1" r="A8" t="n">
+      <c r="D9" t="n">
+        <v>11.5</v>
+      </c>
+      <c s="2" r="E9" t="n">
+        <v>40944.958333333336</v>
+      </c>
+      <c s="2" r="F9" t="n">
+        <v>40946.65625</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c s="1" r="A10" t="n">
         <v>8</v>
       </c>
-      <c s="2" r="B8" t="n">
+      <c s="2" r="B10" t="n">
         <v>40944.958333333336</v>
       </c>
-      <c s="2" r="C8" t="n">
+      <c s="2" r="C10" t="n">
         <v>40946.8125</v>
       </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c s="1" r="A9" t="n">
+      <c r="D10" t="n">
+        <v>40.75</v>
+      </c>
+      <c s="2" r="E10" t="n">
+        <v>40946.65625</v>
+      </c>
+      <c s="2" r="F10" t="n">
+        <v>40946.8125</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c s="1" r="A11" t="n">
         <v>10</v>
       </c>
-      <c s="2" r="B9" t="n">
+      <c s="2" r="B11" t="n">
         <v>40962.875</v>
       </c>
-      <c s="2" r="C9" t="n">
+      <c s="2" r="C11" t="n">
         <v>40963.21875</v>
       </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c s="1" r="A10" t="n">
+      <c r="D11" t="n">
+        <v>8.25</v>
+      </c>
+      <c s="2" r="E11" t="n">
+        <v>40977.25</v>
+      </c>
+      <c s="2" r="F11" t="n">
+        <v>40977.479166666664</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c s="1" r="A12" t="n">
         <v>11</v>
       </c>
-      <c s="2" r="B10" t="n">
+      <c s="2" r="B12" t="n">
         <v>40977.25</v>
       </c>
-      <c s="2" r="C10" t="n">
+      <c s="2" r="C12" t="n">
         <v>40977.479166666664</v>
       </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c s="1" r="A11" t="n">
+      <c r="D12" t="n">
+        <v>5.5</v>
+      </c>
+      <c s="2" r="E12" t="n">
+        <v>40984.520833333336</v>
+      </c>
+      <c s="2" r="F12" t="n">
+        <v>40984.677083333336</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c s="1" r="A13" t="n">
         <v>12</v>
       </c>
-      <c s="2" r="B11" t="n">
+      <c s="2" r="B13" t="n">
         <v>40984.520833333336</v>
       </c>
-      <c s="2" r="C11" t="n">
+      <c s="2" r="C13" t="n">
         <v>40984.677083333336</v>
       </c>
-    </row>
-    <row r="12" spans="1:3">
-      <c s="1" r="A12" t="n">
+      <c r="D13" t="n">
+        <v>3.75</v>
+      </c>
+      <c s="2" r="E13" t="n">
+        <v>40985.489583333336</v>
+      </c>
+      <c s="2" r="F13" t="n">
+        <v>40985.739583333336</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c s="1" r="A14" t="n">
         <v>13</v>
       </c>
-      <c s="2" r="B12" t="n">
+      <c s="2" r="B14" t="n">
         <v>40985.489583333336</v>
       </c>
-      <c s="2" r="C12" t="n">
+      <c s="2" r="C14" t="n">
         <v>40985.739583333336</v>
       </c>
-    </row>
-    <row r="13" spans="1:3">
-      <c s="1" r="A13" t="n">
+      <c r="D14" t="n">
+        <v>6.0</v>
+      </c>
+      <c s="2" r="E14" t="n">
+        <v>40989.84375</v>
+      </c>
+      <c s="2" r="F14" t="n">
+        <v>40990.145833333336</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c s="1" r="A15" t="n">
         <v>14</v>
       </c>
-      <c s="2" r="B13" t="n">
+      <c s="2" r="B15" t="n">
         <v>40989.84375</v>
       </c>
-      <c s="2" r="C13" t="n">
+      <c s="2" r="C15" t="n">
+        <v>40990.145833333336</v>
+      </c>
+      <c r="D15" t="n">
+        <v>7.25</v>
+      </c>
+      <c s="2" r="E15" t="n">
+        <v>40990.21875</v>
+      </c>
+      <c s="2" r="F15" t="n">
         <v>40990.302083333336</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
-      <c s="1" r="A14" t="n">
+    <row r="16" spans="1:6">
+      <c s="1" r="A16" t="n">
+        <v>15</v>
+      </c>
+      <c s="2" r="B16" t="n">
+        <v>40990.21875</v>
+      </c>
+      <c s="2" r="C16" t="n">
+        <v>40990.302083333336</v>
+      </c>
+      <c r="D16" t="n">
+        <v>2.0</v>
+      </c>
+      <c s="2" r="E16" t="n">
+        <v>40990.90625</v>
+      </c>
+      <c s="2" r="F16" t="n">
+        <v>40991.322916666664</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c s="1" r="A17" t="n">
         <v>16</v>
       </c>
-      <c s="2" r="B14" t="n">
+      <c s="2" r="B17" t="n">
         <v>40990.90625</v>
       </c>
-      <c s="2" r="C14" t="n">
+      <c s="2" r="C17" t="n">
         <v>40991.322916666664</v>
       </c>
-    </row>
-    <row r="15" spans="1:3">
-      <c s="1" r="A15" t="n">
+      <c r="D17" t="n">
+        <v>10.0</v>
+      </c>
+      <c s="2" r="E17" t="n">
+        <v>40993.145833333336</v>
+      </c>
+      <c s="2" r="F17" t="n">
+        <v>40993.9375</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c s="1" r="A18" t="n">
         <v>17</v>
       </c>
-      <c s="2" r="B15" t="n">
+      <c s="2" r="B18" t="n">
         <v>40993.145833333336</v>
       </c>
-      <c s="2" r="C15" t="n">
+      <c s="2" r="C18" t="n">
         <v>40993.9375</v>
       </c>
-    </row>
-    <row r="16" spans="1:3">
-      <c s="1" r="A16" t="n">
+      <c r="D18" t="n">
+        <v>19.0</v>
+      </c>
+      <c s="2" r="E18" t="n">
+        <v>41037.197916666664</v>
+      </c>
+      <c s="2" r="F18" t="n">
+        <v>41037.322916666664</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c s="1" r="A19" t="n">
         <v>18</v>
       </c>
-      <c s="2" r="B16" t="n">
+      <c s="2" r="B19" t="n">
         <v>41037.197916666664</v>
       </c>
-      <c s="2" r="C16" t="n">
+      <c s="2" r="C19" t="n">
         <v>41037.322916666664</v>
       </c>
-    </row>
-    <row r="17" spans="1:3">
-      <c s="1" r="A17" t="n">
+      <c r="D19" t="n">
+        <v>3.0</v>
+      </c>
+      <c s="2" r="E19" t="n">
+        <v>41051.78125</v>
+      </c>
+      <c s="2" r="F19" t="n">
+        <v>41052.125</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c s="1" r="A20" t="n">
         <v>19</v>
       </c>
-      <c s="2" r="B17" t="n">
+      <c s="2" r="B20" t="n">
         <v>41051.78125</v>
       </c>
-      <c s="2" r="C17" t="n">
+      <c s="2" r="C20" t="n">
         <v>41052.125</v>
       </c>
-    </row>
-    <row r="18" spans="1:3">
-      <c s="1" r="A18" t="n">
+      <c r="D20" t="n">
+        <v>8.25</v>
+      </c>
+      <c s="2" r="E20" t="n">
+        <v>41052.322916666664</v>
+      </c>
+      <c s="2" r="F20" t="n">
+        <v>41053.5625</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c s="1" r="A21" t="n">
         <v>20</v>
       </c>
-      <c s="2" r="B18" t="n">
+      <c s="2" r="B21" t="n">
         <v>41052.322916666664</v>
       </c>
-      <c s="2" r="C18" t="n">
-        <v>41052.458333333336</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
-      <c s="1" r="A19" t="n">
-        <v>99</v>
-      </c>
-      <c s="2" r="B19" t="n">
-        <v>41052.59375</v>
-      </c>
-      <c s="2" r="C19" t="n">
+      <c s="2" r="C21" t="n">
         <v>41053.5625</v>
       </c>
-    </row>
-    <row r="20" spans="1:3">
-      <c s="1" r="A20" t="n">
+      <c r="D21" t="n">
+        <v>29.75</v>
+      </c>
+      <c s="2" r="E21" t="n">
+        <v>41053.833333333336</v>
+      </c>
+      <c s="2" r="F21" t="n">
+        <v>41054.708333333336</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c s="1" r="A22" t="n">
         <v>21</v>
       </c>
-      <c s="2" r="B20" t="n">
+      <c s="2" r="B22" t="n">
         <v>41053.833333333336</v>
       </c>
-      <c s="2" r="C20" t="n">
+      <c s="2" r="C22" t="n">
         <v>41054.708333333336</v>
       </c>
-    </row>
-    <row r="21" spans="1:3">
-      <c s="1" r="A21" t="n">
+      <c r="D22" t="n">
+        <v>21.0</v>
+      </c>
+      <c s="2" r="E22" t="n">
+        <v>41055.0625</v>
+      </c>
+      <c s="2" r="F22" t="n">
+        <v>41055.697916666664</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c s="1" r="A23" t="n">
         <v>22</v>
       </c>
-      <c s="2" r="B21" t="n">
+      <c s="2" r="B23" t="n">
         <v>41055.0625</v>
       </c>
-      <c s="2" r="C21" t="n">
+      <c s="2" r="C23" t="n">
         <v>41055.697916666664</v>
       </c>
-    </row>
-    <row r="22" spans="1:3">
-      <c s="1" r="A22" t="n">
+      <c r="D23" t="n">
+        <v>15.25</v>
+      </c>
+      <c s="2" r="E23" t="n">
+        <v>41063.427083333336</v>
+      </c>
+      <c s="2" r="F23" t="n">
+        <v>41063.885416666664</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c s="1" r="A24" t="n">
         <v>23</v>
       </c>
-      <c s="2" r="B22" t="n">
+      <c s="2" r="B24" t="n">
         <v>41063.427083333336</v>
       </c>
-      <c s="2" r="C22" t="n">
+      <c s="2" r="C24" t="n">
         <v>41063.885416666664</v>
       </c>
-    </row>
-    <row r="23" spans="1:3">
-      <c s="1" r="A23" t="n">
+      <c r="D24" t="n">
+        <v>11.0</v>
+      </c>
+      <c s="2" r="E24" t="n">
+        <v>41064.010416666664</v>
+      </c>
+      <c s="2" r="F24" t="n">
+        <v>41064.46875</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c s="1" r="A25" t="n">
         <v>24</v>
       </c>
-      <c s="2" r="B23" t="n">
+      <c s="2" r="B25" t="n">
         <v>41064.010416666664</v>
       </c>
-      <c s="2" r="C23" t="n">
+      <c s="2" r="C25" t="n">
         <v>41064.46875</v>
       </c>
-    </row>
-    <row r="24" spans="1:3">
-      <c s="1" r="A24" t="n">
+      <c r="D25" t="n">
+        <v>11.0</v>
+      </c>
+      <c s="2" r="E25" t="n">
+        <v>41064.604166666664</v>
+      </c>
+      <c s="2" r="F25" t="n">
+        <v>41065.875</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c s="1" r="A26" t="n">
         <v>25</v>
       </c>
-      <c s="2" r="B24" t="n">
+      <c s="2" r="B26" t="n">
         <v>41064.604166666664</v>
       </c>
-      <c s="2" r="C24" t="n">
+      <c s="2" r="C26" t="n">
         <v>41065.875</v>
       </c>
-    </row>
-    <row r="25" spans="1:3">
-      <c s="1" r="A25" t="n">
+      <c r="D26" t="n">
+        <v>30.5</v>
+      </c>
+      <c s="2" r="E26" t="n">
+        <v>41066.885416666664</v>
+      </c>
+      <c s="2" r="F26" t="n">
+        <v>41067.15625</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c s="1" r="A27" t="n">
         <v>26</v>
       </c>
-      <c s="2" r="B25" t="n">
+      <c s="2" r="B27" t="n">
         <v>41066.885416666664</v>
       </c>
-      <c s="2" r="C25" t="n">
+      <c s="2" r="C27" t="n">
         <v>41067.15625</v>
       </c>
-    </row>
-    <row r="26" spans="1:3">
-      <c s="1" r="A26" t="n">
+      <c r="D27" t="n">
+        <v>6.5</v>
+      </c>
+      <c s="2" r="E27" t="n">
+        <v>41067.322916666664</v>
+      </c>
+      <c s="2" r="F27" t="n">
+        <v>41067.729166666664</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c s="1" r="A28" t="n">
         <v>27</v>
       </c>
-      <c s="2" r="B26" t="n">
+      <c s="2" r="B28" t="n">
         <v>41067.322916666664</v>
       </c>
-      <c s="2" r="C26" t="n">
+      <c s="2" r="C28" t="n">
         <v>41067.729166666664</v>
       </c>
-    </row>
-    <row r="27" spans="1:3">
-      <c s="1" r="A27" t="n">
+      <c r="D28" t="n">
+        <v>9.75</v>
+      </c>
+      <c s="2" r="E28" t="n">
+        <v>41098.083333333336</v>
+      </c>
+      <c s="2" r="F28" t="n">
+        <v>41098.25</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c s="1" r="A29" t="n">
         <v>28</v>
       </c>
-      <c s="2" r="B27" t="n">
+      <c s="2" r="B29" t="n">
         <v>41098.083333333336</v>
       </c>
-      <c s="2" r="C27" t="n">
+      <c s="2" r="C29" t="n">
         <v>41098.25</v>
       </c>
-    </row>
-    <row r="28" spans="1:3">
-      <c s="1" r="A28" t="n">
+      <c r="D29" t="n">
+        <v>4.0</v>
+      </c>
+      <c s="2" r="E29" t="n">
+        <v>41130.145833333336</v>
+      </c>
+      <c s="2" r="F29" t="n">
+        <v>41130.364583333336</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c s="1" r="A30" t="n">
         <v>29</v>
       </c>
-      <c s="2" r="B28" t="n">
+      <c s="2" r="B30" t="n">
         <v>41130.145833333336</v>
       </c>
-      <c s="2" r="C28" t="n">
+      <c s="2" r="C30" t="n">
         <v>41130.364583333336</v>
       </c>
-    </row>
-    <row r="29" spans="1:3">
-      <c s="1" r="A29" t="n">
+      <c r="D30" t="n">
+        <v>5.25</v>
+      </c>
+      <c s="2" r="E30" t="n">
+        <v>41153.479166666664</v>
+      </c>
+      <c s="2" r="F30" t="n">
+        <v>41153.78125</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
+      <c s="1" r="A31" t="n">
         <v>30</v>
       </c>
-      <c s="2" r="B29" t="n">
+      <c s="2" r="B31" t="n">
         <v>41153.479166666664</v>
       </c>
-      <c s="2" r="C29" t="n">
+      <c s="2" r="C31" t="n">
         <v>41153.78125</v>
       </c>
-    </row>
-    <row r="30" spans="1:3">
-      <c s="1" r="A30" t="n">
+      <c r="D31" t="n">
+        <v>7.25</v>
+      </c>
+      <c s="2" r="E31" t="n">
+        <v>41153.791666666664</v>
+      </c>
+      <c s="2" r="F31" t="n">
+        <v>41155.135416666664</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
+      <c s="1" r="A32" t="n">
         <v>31</v>
       </c>
-      <c s="2" r="B30" t="n">
+      <c s="2" r="B32" t="n">
         <v>41153.791666666664</v>
       </c>
-      <c s="2" r="C30" t="n">
+      <c s="2" r="C32" t="n">
         <v>41155.135416666664</v>
       </c>
-    </row>
-    <row r="31" spans="1:3">
-      <c s="1" r="A31" t="n">
+      <c r="D32" t="n">
+        <v>32.25</v>
+      </c>
+      <c s="2" r="E32" t="n">
+        <v>41316.864583333336</v>
+      </c>
+      <c s="2" r="F32" t="n">
+        <v>41317.53125</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
+      <c s="1" r="A33" t="n">
         <v>32</v>
       </c>
-      <c s="2" r="B31" t="n">
+      <c s="2" r="B33" t="n">
         <v>41316.864583333336</v>
       </c>
-      <c s="2" r="C31" t="n">
+      <c s="2" r="C33" t="n">
         <v>41317.53125</v>
       </c>
-    </row>
-    <row r="32" spans="1:3">
-      <c s="1" r="A32" t="n">
+      <c r="D33" t="n">
+        <v>16.0</v>
+      </c>
+      <c s="2" r="E33" t="n">
+        <v>41338.770833333336</v>
+      </c>
+      <c s="2" r="F33" t="n">
+        <v>41339.09375</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
+      <c s="1" r="A34" t="n">
         <v>33</v>
       </c>
-      <c s="2" r="B32" t="n">
+      <c s="2" r="B34" t="n">
         <v>41338.770833333336</v>
       </c>
-      <c s="2" r="C32" t="n">
+      <c s="2" r="C34" t="n">
         <v>41339.09375</v>
       </c>
-    </row>
-    <row r="33" spans="1:3">
-      <c s="1" r="A33" t="n">
+      <c r="D34" t="n">
+        <v>7.75</v>
+      </c>
+      <c s="2" r="E34" t="n">
+        <v>41339.375</v>
+      </c>
+      <c s="2" r="F34" t="n">
+        <v>41339.947916666664</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
+      <c s="1" r="A35" t="n">
         <v>34</v>
       </c>
-      <c s="2" r="B33" t="n">
+      <c s="2" r="B35" t="n">
         <v>41339.375</v>
       </c>
-      <c s="2" r="C33" t="n">
+      <c s="2" r="C35" t="n">
         <v>41339.947916666664</v>
       </c>
-    </row>
-    <row r="34" spans="1:3">
-      <c s="1" r="A34" t="n">
+      <c r="D35" t="n">
+        <v>13.75</v>
+      </c>
+      <c s="2" r="E35" t="n">
+        <v>41340.583333333336</v>
+      </c>
+      <c s="2" r="F35" t="n">
+        <v>41341.916666666664</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
+      <c s="1" r="A36" t="n">
         <v>35</v>
       </c>
-      <c s="2" r="B34" t="n">
+      <c s="2" r="B36" t="n">
         <v>41340.583333333336</v>
       </c>
-      <c s="2" r="C34" t="n">
+      <c s="2" r="C36" t="n">
         <v>41341.916666666664</v>
       </c>
-    </row>
-    <row r="35" spans="1:3">
-      <c s="1" r="A35" t="n">
+      <c r="D36" t="n">
+        <v>32.0</v>
+      </c>
+      <c s="2" r="E36" t="n">
+        <v>41344.083333333336</v>
+      </c>
+      <c s="2" r="F36" t="n">
+        <v>41344.833333333336</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
+      <c s="1" r="A37" t="n">
         <v>36</v>
       </c>
-      <c s="2" r="B35" t="n">
+      <c s="2" r="B37" t="n">
         <v>41344.083333333336</v>
       </c>
-      <c s="2" r="C35" t="n">
+      <c s="2" r="C37" t="n">
         <v>41344.833333333336</v>
       </c>
-    </row>
-    <row r="36" spans="1:3">
-      <c s="1" r="A36" t="n">
+      <c r="D37" t="n">
+        <v>18.0</v>
+      </c>
+      <c s="2" r="E37" t="n">
+        <v>41354.541666666664</v>
+      </c>
+      <c s="2" r="F37" t="n">
+        <v>41354.635416666664</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
+      <c s="1" r="A38" t="n">
         <v>37</v>
       </c>
-      <c s="2" r="B36" t="n">
+      <c s="2" r="B38" t="n">
         <v>41354.541666666664</v>
       </c>
-      <c s="2" r="C36" t="n">
+      <c s="2" r="C38" t="n">
         <v>41354.635416666664</v>
       </c>
-    </row>
-    <row r="37" spans="1:3">
-      <c s="1" r="A37" t="n">
+      <c r="D38" t="n">
+        <v>2.25</v>
+      </c>
+      <c s="2" r="E38" t="n">
+        <v>41356.447916666664</v>
+      </c>
+      <c s="2" r="F38" t="n">
+        <v>41356.520833333336</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
+      <c s="1" r="A39" t="n">
         <v>38</v>
       </c>
-      <c s="2" r="B37" t="n">
+      <c s="2" r="B39" t="n">
         <v>41356.447916666664</v>
       </c>
-      <c s="2" r="C37" t="n">
+      <c s="2" r="C39" t="n">
         <v>41356.520833333336</v>
       </c>
-    </row>
-    <row r="38" spans="1:3">
-      <c s="1" r="A38" t="n">
+      <c r="D39" t="n">
+        <v>1.75</v>
+      </c>
+      <c s="2" r="E39" t="n">
+        <v>41380.447916666664</v>
+      </c>
+      <c s="2" r="F39" t="n">
+        <v>41381.947916666664</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
+      <c s="1" r="A40" t="n">
         <v>39</v>
       </c>
-      <c s="2" r="B38" t="n">
+      <c s="2" r="B40" t="n">
         <v>41380.447916666664</v>
       </c>
-      <c s="2" r="C38" t="n">
+      <c s="2" r="C40" t="n">
         <v>41381.947916666664</v>
       </c>
-    </row>
-    <row r="39" spans="1:3">
-      <c s="1" r="A39" t="n">
+      <c r="D40" t="n">
+        <v>36.0</v>
+      </c>
+      <c s="2" r="E40" t="n">
+        <v>41382.625</v>
+      </c>
+      <c s="2" r="F40" t="n">
+        <v>41382.697916666664</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
+      <c s="1" r="A41" t="n">
         <v>40</v>
       </c>
-      <c s="2" r="B39" t="n">
+      <c s="2" r="B41" t="n">
         <v>41382.625</v>
       </c>
-      <c s="2" r="C39" t="n">
+      <c s="2" r="C41" t="n">
         <v>41382.697916666664</v>
       </c>
-    </row>
-    <row r="40" spans="1:3">
-      <c s="1" r="A40" t="n">
+      <c r="D41" t="n">
+        <v>1.75</v>
+      </c>
+      <c s="2" r="E41" t="n">
+        <v>41382.791666666664</v>
+      </c>
+      <c s="2" r="F41" t="n">
+        <v>41382.979166666664</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6">
+      <c s="1" r="A42" t="n">
         <v>41</v>
       </c>
-      <c s="2" r="B40" t="n">
+      <c s="2" r="B42" t="n">
         <v>41382.791666666664</v>
       </c>
-      <c s="2" r="C40" t="n">
+      <c s="2" r="C42" t="n">
         <v>41382.979166666664</v>
       </c>
-    </row>
-    <row r="41" spans="1:3">
-      <c s="1" r="A41" t="n">
+      <c r="D42" t="n">
+        <v>4.5</v>
+      </c>
+      <c s="2" r="E42" t="n">
+        <v>41384.15625</v>
+      </c>
+      <c s="2" r="F42" t="n">
+        <v>41384.9375</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6">
+      <c s="1" r="A43" t="n">
         <v>42</v>
       </c>
-      <c s="2" r="B41" t="n">
+      <c s="2" r="B43" t="n">
         <v>41384.15625</v>
       </c>
-      <c s="2" r="C41" t="n">
+      <c s="2" r="C43" t="n">
         <v>41384.9375</v>
       </c>
-    </row>
-    <row r="42" spans="1:3">
-      <c s="1" r="A42" t="n">
+      <c r="D43" t="n">
+        <v>18.75</v>
+      </c>
+      <c s="2" r="E43" t="n">
+        <v>41387.541666666664</v>
+      </c>
+      <c s="2" r="F43" t="n">
+        <v>41388.947916666664</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6">
+      <c s="1" r="A44" t="n">
         <v>43</v>
       </c>
-      <c s="2" r="B42" t="n">
+      <c s="2" r="B44" t="n">
         <v>41387.541666666664</v>
       </c>
-      <c s="2" r="C42" t="n">
+      <c s="2" r="C44" t="n">
         <v>41388.947916666664</v>
       </c>
-    </row>
-    <row r="43" spans="1:3">
-      <c s="1" r="A43" t="n">
+      <c r="D44" t="n">
+        <v>33.75</v>
+      </c>
+      <c s="2" r="E44" t="n">
+        <v>41392.083333333336</v>
+      </c>
+      <c s="2" r="F44" t="n">
+        <v>41392.177083333336</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6">
+      <c s="1" r="A45" t="n">
         <v>44</v>
       </c>
-      <c s="2" r="B43" t="n">
+      <c s="2" r="B45" t="n">
         <v>41392.083333333336</v>
       </c>
-      <c s="2" r="C43" t="n">
+      <c s="2" r="C45" t="n">
         <v>41392.177083333336</v>
       </c>
-    </row>
-    <row r="44" spans="1:3">
-      <c s="1" r="A44" t="n">
+      <c r="D45" t="n">
+        <v>2.25</v>
+      </c>
+      <c s="2" r="E45" t="n">
+        <v>41392.40625</v>
+      </c>
+      <c s="2" r="F45" t="n">
+        <v>41393.822916666664</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6">
+      <c s="1" r="A46" t="n">
         <v>45</v>
       </c>
-      <c s="2" r="B44" t="n">
+      <c s="2" r="B46" t="n">
         <v>41392.40625</v>
       </c>
-      <c s="2" r="C44" t="n">
+      <c s="2" r="C46" t="n">
         <v>41393.822916666664</v>
       </c>
-    </row>
-    <row r="45" spans="1:3">
-      <c s="1" r="A45" t="n">
+      <c r="D46" t="n">
+        <v>34.0</v>
+      </c>
+      <c s="2" r="E46" t="n">
+        <v>41394.59375</v>
+      </c>
+      <c s="2" r="F46" t="n">
+        <v>41396.15625</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6">
+      <c s="1" r="A47" t="n">
+        <v>46</v>
+      </c>
+      <c s="2" r="B47" t="n">
+        <v>41394.59375</v>
+      </c>
+      <c s="2" r="C47" t="n">
+        <v>41396.15625</v>
+      </c>
+      <c r="D47" t="n">
+        <v>37.5</v>
+      </c>
+      <c s="2" r="E47" t="n">
+        <v>41405.59375</v>
+      </c>
+      <c s="2" r="F47" t="n">
+        <v>41405.833333333336</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6">
+      <c s="1" r="A48" t="n">
         <v>47</v>
       </c>
-      <c s="2" r="B45" t="n">
+      <c s="2" r="B48" t="n">
         <v>41405.59375</v>
       </c>
-      <c s="2" r="C45" t="n">
+      <c s="2" r="C48" t="n">
         <v>41405.833333333336</v>
       </c>
-    </row>
-    <row r="46" spans="1:3">
-      <c s="1" r="A46" t="n">
+      <c r="D48" t="n">
+        <v>5.75</v>
+      </c>
+      <c s="2" r="E48" t="n">
+        <v>41430.135416666664</v>
+      </c>
+      <c s="2" r="F48" t="n">
+        <v>41431.854166666664</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6">
+      <c s="1" r="A49" t="n">
+        <v>48</v>
+      </c>
+      <c s="2" r="B49" t="n">
+        <v>41430.135416666664</v>
+      </c>
+      <c s="2" r="C49" t="n">
+        <v>41431.854166666664</v>
+      </c>
+      <c r="D49" t="n">
+        <v>41.25</v>
+      </c>
+      <c s="2" r="E49" t="n">
+        <v>41441.114583333336</v>
+      </c>
+      <c s="2" r="F49" t="n">
+        <v>41441.729166666664</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6">
+      <c s="1" r="A50" t="n">
         <v>49</v>
       </c>
-      <c s="2" r="B46" t="n">
+      <c s="2" r="B50" t="n">
         <v>41441.114583333336</v>
       </c>
-      <c s="2" r="C46" t="n">
+      <c s="2" r="C50" t="n">
         <v>41441.729166666664</v>
       </c>
-    </row>
-    <row r="47" spans="1:3">
-      <c s="1" r="A47" t="n">
+      <c r="D50" t="n">
+        <v>14.75</v>
+      </c>
+      <c s="2" r="E50" t="n">
+        <v>41468.708333333336</v>
+      </c>
+      <c s="2" r="F50" t="n">
+        <v>41468.833333333336</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6">
+      <c s="1" r="A51" t="n">
         <v>50</v>
       </c>
-      <c s="2" r="B47" t="n">
+      <c s="2" r="B51" t="n">
         <v>41468.708333333336</v>
       </c>
-      <c s="2" r="C47" t="n">
+      <c s="2" r="C51" t="n">
         <v>41468.833333333336</v>
       </c>
-    </row>
-    <row r="48" spans="1:3">
-      <c s="1" r="A48" t="n">
+      <c r="D51" t="n">
+        <v>3.0</v>
+      </c>
+      <c s="2" r="E51" t="n">
+        <v>41472.135416666664</v>
+      </c>
+      <c s="2" r="F51" t="n">
+        <v>41472.322916666664</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6">
+      <c s="1" r="A52" t="n">
         <v>51</v>
       </c>
-      <c s="2" r="B48" t="n">
+      <c s="2" r="B52" t="n">
         <v>41472.135416666664</v>
       </c>
-      <c s="2" r="C48" t="n">
+      <c s="2" r="C52" t="n">
         <v>41472.322916666664</v>
       </c>
-    </row>
-    <row r="49" spans="1:3">
-      <c s="1" r="A49" t="n">
+      <c r="D52" t="n">
+        <v>4.5</v>
+      </c>
+      <c s="2" r="E52" t="n">
+        <v>41472.947916666664</v>
+      </c>
+      <c s="2" r="F52" t="n">
+        <v>41473.729166666664</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6">
+      <c s="1" r="A53" t="n">
         <v>52</v>
       </c>
-      <c s="2" r="B49" t="n">
+      <c s="2" r="B53" t="n">
         <v>41472.947916666664</v>
       </c>
-      <c s="2" r="C49" t="n">
+      <c s="2" r="C53" t="n">
         <v>41473.729166666664</v>
       </c>
-    </row>
-    <row r="50" spans="1:3">
-      <c s="1" r="A50" t="n">
+      <c r="D53" t="n">
+        <v>18.75</v>
+      </c>
+      <c s="2" r="E53" t="n">
+        <v>41474.0625</v>
+      </c>
+      <c s="2" r="F53" t="n">
+        <v>41475.9375</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6">
+      <c s="1" r="A54" t="n">
         <v>53</v>
       </c>
-      <c s="2" r="B50" t="n">
+      <c s="2" r="B54" t="n">
         <v>41474.0625</v>
       </c>
-      <c s="2" r="C50" t="n">
+      <c s="2" r="C54" t="n">
         <v>41475.9375</v>
       </c>
-    </row>
-    <row r="51" spans="1:3">
-      <c s="1" r="A51" t="n">
+      <c r="D54" t="n">
+        <v>45.0</v>
+      </c>
+      <c s="2" r="E54" t="n">
+        <v>41482.9375</v>
+      </c>
+      <c s="2" r="F54" t="n">
+        <v>41483.135416666664</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6">
+      <c s="1" r="A55" t="n">
         <v>54</v>
       </c>
-      <c s="2" r="B51" t="n">
+      <c s="2" r="B55" t="n">
         <v>41482.9375</v>
       </c>
-      <c s="2" r="C51" t="n">
+      <c s="2" r="C55" t="n">
         <v>41483.135416666664</v>
       </c>
-    </row>
-    <row r="52" spans="1:3">
-      <c s="1" r="A52" t="n">
+      <c r="D55" t="n">
+        <v>4.75</v>
+      </c>
+      <c s="2" r="E55" t="n">
+        <v>41489.666666666664</v>
+      </c>
+      <c s="2" r="F55" t="n">
+        <v>41489.802083333336</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6">
+      <c s="1" r="A56" t="n">
         <v>55</v>
       </c>
-      <c s="2" r="B52" t="n">
+      <c s="2" r="B56" t="n">
         <v>41489.666666666664</v>
       </c>
-      <c s="2" r="C52" t="n">
+      <c s="2" r="C56" t="n">
         <v>41489.802083333336</v>
       </c>
-    </row>
-    <row r="53" spans="1:3">
-      <c s="1" r="A53" t="n">
+      <c r="D56" t="n">
+        <v>3.25</v>
+      </c>
+      <c s="2" r="E56" t="n">
+        <v>41491.9375</v>
+      </c>
+      <c s="2" r="F56" t="n">
+        <v>41492.416666666664</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6">
+      <c s="1" r="A57" t="n">
         <v>56</v>
       </c>
-      <c s="2" r="B53" t="n">
+      <c s="2" r="B57" t="n">
         <v>41491.9375</v>
       </c>
-      <c s="2" r="C53" t="n">
+      <c s="2" r="C57" t="n">
         <v>41492.416666666664</v>
       </c>
-    </row>
-    <row r="54" spans="1:3">
-      <c s="1" r="A54" t="n">
+      <c r="D57" t="n">
+        <v>11.5</v>
+      </c>
+      <c s="2" r="E57" t="n">
+        <v>41496.177083333336</v>
+      </c>
+      <c s="2" r="F57" t="n">
+        <v>41497.135416666664</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6">
+      <c s="1" r="A58" t="n">
         <v>57</v>
       </c>
-      <c s="2" r="B54" t="n">
+      <c s="2" r="B58" t="n">
         <v>41496.177083333336</v>
       </c>
-      <c s="2" r="C54" t="n">
+      <c s="2" r="C58" t="n">
         <v>41497.135416666664</v>
       </c>
-    </row>
-    <row r="55" spans="1:3">
-      <c s="1" r="A55" t="n">
+      <c r="D58" t="n">
+        <v>23.0</v>
+      </c>
+      <c s="2" r="E58" t="n">
+        <v>41501.78125</v>
+      </c>
+      <c s="2" r="F58" t="n">
+        <v>41501.958333333336</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6">
+      <c s="1" r="A59" t="n">
         <v>58</v>
       </c>
-      <c s="2" r="B55" t="n">
+      <c s="2" r="B59" t="n">
         <v>41501.78125</v>
       </c>
-      <c s="2" r="C55" t="n">
+      <c s="2" r="C59" t="n">
         <v>41501.958333333336</v>
       </c>
-    </row>
-    <row r="56" spans="1:3">
-      <c s="1" r="A56" t="n">
+      <c r="D59" t="n">
+        <v>4.25</v>
+      </c>
+      <c s="2" r="E59" t="n">
+        <v>41502.322916666664</v>
+      </c>
+      <c s="2" r="F59" t="n">
+        <v>41504.572916666664</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6">
+      <c s="1" r="A60" t="n">
         <v>59</v>
       </c>
-      <c s="2" r="B56" t="n">
+      <c s="2" r="B60" t="n">
         <v>41502.322916666664</v>
       </c>
-      <c s="2" r="C56" t="n">
-        <v>41503.25</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3">
-      <c s="1" r="A57" t="n">
-        <v>999</v>
-      </c>
-      <c s="2" r="B57" t="n">
-        <v>41503.458333333336</v>
-      </c>
-      <c s="2" r="C57" t="n">
+      <c s="2" r="C60" t="n">
         <v>41504.572916666664</v>
       </c>
-    </row>
-    <row r="58" spans="1:3">
-      <c s="1" r="A58" t="n">
+      <c r="D60" t="n">
+        <v>54.0</v>
+      </c>
+      <c s="2" r="E60" t="n">
+        <v>41505.270833333336</v>
+      </c>
+      <c s="2" r="F60" t="n">
+        <v>41505.854166666664</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6">
+      <c s="1" r="A61" t="n">
         <v>60</v>
       </c>
-      <c s="2" r="B58" t="n">
+      <c s="2" r="B61" t="n">
         <v>41505.270833333336</v>
       </c>
-      <c s="2" r="C58" t="n">
+      <c s="2" r="C61" t="n">
         <v>41505.854166666664</v>
       </c>
-    </row>
-    <row r="59" spans="1:3">
-      <c s="1" r="A59" t="n">
+      <c r="D61" t="n">
+        <v>14.0</v>
+      </c>
+      <c s="2" r="E61" t="n">
+        <v>41518.1875</v>
+      </c>
+      <c s="2" r="F61" t="n">
+        <v>41518.260416666664</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6">
+      <c s="1" r="A62" t="n">
         <v>61</v>
       </c>
-      <c s="2" r="B59" t="n">
+      <c s="2" r="B62" t="n">
         <v>41518.1875</v>
       </c>
-      <c s="2" r="C59" t="n">
+      <c s="2" r="C62" t="n">
         <v>41518.260416666664</v>
       </c>
-    </row>
-    <row r="60" spans="1:3">
-      <c s="1" r="A60" t="n">
+      <c r="D62" t="n">
+        <v>1.75</v>
+      </c>
+      <c s="2" r="E62" t="n">
+        <v>41518.34375</v>
+      </c>
+      <c s="2" r="F62" t="n">
+        <v>41518.572916666664</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6">
+      <c s="1" r="A63" t="n">
         <v>62</v>
       </c>
-      <c s="2" r="B60" t="n">
+      <c s="2" r="B63" t="n">
         <v>41518.34375</v>
       </c>
-      <c s="2" r="C60" t="n">
+      <c s="2" r="C63" t="n">
         <v>41518.572916666664</v>
       </c>
-    </row>
-    <row r="61" spans="1:3">
-      <c s="1" r="A61" t="n">
+      <c r="D63" t="n">
+        <v>5.5</v>
+      </c>
+      <c s="2" r="E63" t="n">
+        <v>41684.625</v>
+      </c>
+      <c s="2" r="F63" t="n">
+        <v>41684.8125</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6">
+      <c s="1" r="A64" t="n">
         <v>63</v>
       </c>
-      <c s="2" r="B61" t="n">
+      <c s="2" r="B64" t="n">
         <v>41684.625</v>
       </c>
-      <c s="2" r="C61" t="n">
+      <c s="2" r="C64" t="n">
         <v>41684.8125</v>
       </c>
-    </row>
-    <row r="62" spans="1:3">
-      <c s="1" r="A62" t="n">
+      <c r="D64" t="n">
+        <v>4.5</v>
+      </c>
+      <c s="2" r="E64" t="n">
+        <v>41690.46875</v>
+      </c>
+      <c s="2" r="F64" t="n">
+        <v>41690.75</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6">
+      <c s="1" r="A65" t="n">
         <v>64</v>
       </c>
-      <c s="2" r="B62" t="n">
+      <c s="2" r="B65" t="n">
         <v>41690.46875</v>
       </c>
-      <c s="2" r="C62" t="n">
+      <c s="2" r="C65" t="n">
         <v>41690.75</v>
       </c>
-    </row>
-    <row r="63" spans="1:3">
-      <c s="1" r="A63" t="n">
+      <c r="D65" t="n">
+        <v>6.75</v>
+      </c>
+      <c s="2" r="E65" t="n">
+        <v>41691.479166666664</v>
+      </c>
+      <c s="2" r="F65" t="n">
+        <v>41692.145833333336</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6">
+      <c s="1" r="A66" t="n">
         <v>65</v>
       </c>
-      <c s="2" r="B63" t="n">
+      <c s="2" r="B66" t="n">
         <v>41691.479166666664</v>
       </c>
-      <c s="2" r="C63" t="n">
+      <c s="2" r="C66" t="n">
         <v>41692.145833333336</v>
       </c>
-    </row>
-    <row r="64" spans="1:3">
-      <c s="1" r="A64" t="n">
+      <c r="D66" t="n">
+        <v>16.0</v>
+      </c>
+      <c s="2" r="E66" t="n">
+        <v>41695.885416666664</v>
+      </c>
+      <c s="2" r="F66" t="n">
+        <v>41696.677083333336</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6">
+      <c s="1" r="A67" t="n">
         <v>66</v>
       </c>
-      <c s="2" r="B64" t="n">
+      <c s="2" r="B67" t="n">
         <v>41695.885416666664</v>
       </c>
-      <c s="2" r="C64" t="n">
+      <c s="2" r="C67" t="n">
         <v>41696.677083333336</v>
       </c>
-    </row>
-    <row r="65" spans="1:3">
-      <c s="1" r="A65" t="n">
+      <c r="D67" t="n">
+        <v>19.0</v>
+      </c>
+      <c s="2" r="E67" t="n">
+        <v>41697.083333333336</v>
+      </c>
+      <c s="2" r="F67" t="n">
+        <v>41697.53125</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6">
+      <c s="1" r="A68" t="n">
         <v>67</v>
       </c>
-      <c s="2" r="B65" t="n">
+      <c s="2" r="B68" t="n">
         <v>41697.083333333336</v>
       </c>
-      <c s="2" r="C65" t="n">
+      <c s="2" r="C68" t="n">
         <v>41697.53125</v>
       </c>
-    </row>
-    <row r="66" spans="1:3">
-      <c s="1" r="A66" t="n">
+      <c r="D68" t="n">
+        <v>10.75</v>
+      </c>
+      <c s="2" r="E68" t="n">
+        <v>41697.677083333336</v>
+      </c>
+      <c s="2" r="F68" t="n">
+        <v>41698.010416666664</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6">
+      <c s="1" r="A69" t="n">
         <v>68</v>
       </c>
-      <c s="2" r="B66" t="n">
+      <c s="2" r="B69" t="n">
         <v>41697.677083333336</v>
       </c>
-      <c s="2" r="C66" t="n">
+      <c s="2" r="C69" t="n">
         <v>41698.010416666664</v>
       </c>
-    </row>
-    <row r="67" spans="1:3">
-      <c s="1" r="A67" t="n">
+      <c r="D69" t="n">
+        <v>8.0</v>
+      </c>
+      <c s="2" r="E69" t="n">
+        <v>41704.822916666664</v>
+      </c>
+      <c s="2" r="F69" t="n">
+        <v>41705.197916666664</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6">
+      <c s="1" r="A70" t="n">
         <v>69</v>
       </c>
-      <c s="2" r="B67" t="n">
+      <c s="2" r="B70" t="n">
         <v>41704.822916666664</v>
       </c>
-      <c s="2" r="C67" t="n">
+      <c s="2" r="C70" t="n">
         <v>41705.197916666664</v>
       </c>
-    </row>
-    <row r="68" spans="1:3">
-      <c s="1" r="A68" t="n">
+      <c r="D70" t="n">
+        <v>9.0</v>
+      </c>
+      <c s="2" r="E70" t="n">
+        <v>41711.520833333336</v>
+      </c>
+      <c s="2" r="F70" t="n">
+        <v>41711.635416666664</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6">
+      <c s="1" r="A71" t="n">
         <v>70</v>
       </c>
-      <c s="2" r="B68" t="n">
+      <c s="2" r="B71" t="n">
         <v>41711.520833333336</v>
       </c>
-      <c s="2" r="C68" t="n">
+      <c s="2" r="C71" t="n">
+        <v>41711.635416666664</v>
+      </c>
+      <c r="D71" t="n">
+        <v>2.75</v>
+      </c>
+      <c s="2" r="E71" t="n">
+        <v>41711.666666666664</v>
+      </c>
+      <c s="2" r="F71" t="n">
+        <v>41711.791666666664</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6">
+      <c s="1" r="A72" t="n">
+        <v>71</v>
+      </c>
+      <c s="2" r="B72" t="n">
+        <v>41711.666666666664</v>
+      </c>
+      <c s="2" r="C72" t="n">
+        <v>41711.791666666664</v>
+      </c>
+      <c r="D72" t="n">
+        <v>3.0</v>
+      </c>
+      <c s="2" r="E72" t="n">
+        <v>41711.833333333336</v>
+      </c>
+      <c s="2" r="F72" t="n">
         <v>41711.927083333336</v>
       </c>
     </row>
-    <row r="69" spans="1:3">
-      <c s="1" r="A69" t="n">
+    <row r="73" spans="1:6">
+      <c s="1" r="A73" t="n">
+        <v>72</v>
+      </c>
+      <c s="2" r="B73" t="n">
+        <v>41711.833333333336</v>
+      </c>
+      <c s="2" r="C73" t="n">
+        <v>41711.927083333336</v>
+      </c>
+      <c r="D73" t="n">
+        <v>2.25</v>
+      </c>
+      <c s="2" r="E73" t="n">
+        <v>41712.020833333336</v>
+      </c>
+      <c s="2" r="F73" t="n">
+        <v>41712.34375</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6">
+      <c s="1" r="A74" t="n">
         <v>73</v>
       </c>
-      <c s="2" r="B69" t="n">
+      <c s="2" r="B74" t="n">
         <v>41712.020833333336</v>
       </c>
-      <c s="2" r="C69" t="n">
+      <c s="2" r="C74" t="n">
         <v>41712.34375</v>
       </c>
-    </row>
-    <row r="70" spans="1:3">
-      <c s="1" r="A70" t="n">
+      <c r="D74" t="n">
+        <v>7.75</v>
+      </c>
+      <c s="2" r="E74" t="n">
+        <v>41735.520833333336</v>
+      </c>
+      <c s="2" r="F74" t="n">
+        <v>41735.989583333336</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6">
+      <c s="1" r="A75" t="n">
         <v>74</v>
       </c>
-      <c s="2" r="B70" t="n">
+      <c s="2" r="B75" t="n">
         <v>41735.520833333336</v>
       </c>
-      <c s="2" r="C70" t="n">
+      <c s="2" r="C75" t="n">
         <v>41735.989583333336</v>
       </c>
-    </row>
-    <row r="71" spans="1:3">
-      <c s="1" r="A71" t="n">
+      <c r="D75" t="n">
+        <v>11.25</v>
+      </c>
+      <c s="2" r="E75" t="n">
+        <v>41737.604166666664</v>
+      </c>
+      <c s="2" r="F75" t="n">
+        <v>41737.770833333336</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6">
+      <c s="1" r="A76" t="n">
         <v>75</v>
       </c>
-      <c s="2" r="B71" t="n">
+      <c s="2" r="B76" t="n">
         <v>41737.604166666664</v>
       </c>
-      <c s="2" r="C71" t="n">
+      <c s="2" r="C76" t="n">
         <v>41737.770833333336</v>
       </c>
-    </row>
-    <row r="72" spans="1:3">
-      <c s="1" r="A72" t="n">
+      <c r="D76" t="n">
+        <v>4.0</v>
+      </c>
+      <c s="2" r="E76" t="n">
+        <v>41738.989583333336</v>
+      </c>
+      <c s="2" r="F76" t="n">
+        <v>41739.15625</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6">
+      <c s="1" r="A77" t="n">
         <v>76</v>
       </c>
-      <c s="2" r="B72" t="n">
+      <c s="2" r="B77" t="n">
         <v>41738.989583333336</v>
       </c>
-      <c s="2" r="C72" t="n">
+      <c s="2" r="C77" t="n">
         <v>41739.15625</v>
       </c>
-    </row>
-    <row r="73" spans="1:3">
-      <c s="1" r="A73" t="n">
+      <c r="D77" t="n">
+        <v>4.0</v>
+      </c>
+      <c s="2" r="E77" t="n">
+        <v>41747.791666666664</v>
+      </c>
+      <c s="2" r="F77" t="n">
+        <v>41747.958333333336</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6">
+      <c s="1" r="A78" t="n">
         <v>77</v>
       </c>
-      <c s="2" r="B73" t="n">
+      <c s="2" r="B78" t="n">
         <v>41747.791666666664</v>
       </c>
-      <c s="2" r="C73" t="n">
+      <c s="2" r="C78" t="n">
         <v>41747.958333333336</v>
       </c>
-    </row>
-    <row r="74" spans="1:3">
-      <c s="1" r="A74" t="n">
+      <c r="D78" t="n">
+        <v>4.0</v>
+      </c>
+      <c s="2" r="E78" t="n">
+        <v>41748.291666666664</v>
+      </c>
+      <c s="2" r="F78" t="n">
+        <v>41748.927083333336</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6">
+      <c s="1" r="A79" t="n">
         <v>78</v>
       </c>
-      <c s="2" r="B74" t="n">
+      <c s="2" r="B79" t="n">
         <v>41748.291666666664</v>
       </c>
-      <c s="2" r="C74" t="n">
+      <c s="2" r="C79" t="n">
         <v>41748.927083333336</v>
       </c>
-    </row>
-    <row r="75" spans="1:3">
-      <c s="1" r="A75" t="n">
+      <c r="D79" t="n">
+        <v>15.25</v>
+      </c>
+      <c s="2" r="E79" t="n">
+        <v>41748.958333333336</v>
+      </c>
+      <c s="2" r="F79" t="n">
+        <v>41749.40625</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6">
+      <c s="1" r="A80" t="n">
         <v>79</v>
       </c>
-      <c s="2" r="B75" t="n">
+      <c s="2" r="B80" t="n">
         <v>41748.958333333336</v>
       </c>
-      <c s="2" r="C75" t="n">
+      <c s="2" r="C80" t="n">
         <v>41749.40625</v>
       </c>
-    </row>
-    <row r="76" spans="1:3">
-      <c s="1" r="A76" t="n">
+      <c r="D80" t="n">
+        <v>10.75</v>
+      </c>
+      <c s="2" r="E80" t="n">
+        <v>41754.65625</v>
+      </c>
+      <c s="2" r="F80" t="n">
+        <v>41754.791666666664</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6">
+      <c s="1" r="A81" t="n">
         <v>80</v>
       </c>
-      <c s="2" r="B76" t="n">
+      <c s="2" r="B81" t="n">
         <v>41754.65625</v>
       </c>
-      <c s="2" r="C76" t="n">
+      <c s="2" r="C81" t="n">
         <v>41754.791666666664</v>
       </c>
-    </row>
-    <row r="77" spans="1:3">
-      <c s="1" r="A77" t="n">
+      <c r="D81" t="n">
+        <v>3.25</v>
+      </c>
+      <c s="2" r="E81" t="n">
+        <v>41756.489583333336</v>
+      </c>
+      <c s="2" r="F81" t="n">
+        <v>41756.822916666664</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6">
+      <c s="1" r="A82" t="n">
         <v>81</v>
       </c>
-      <c s="2" r="B77" t="n">
+      <c s="2" r="B82" t="n">
         <v>41756.489583333336</v>
       </c>
-      <c s="2" r="C77" t="n">
+      <c s="2" r="C82" t="n">
         <v>41756.822916666664</v>
       </c>
-    </row>
-    <row r="78" spans="1:3">
-      <c s="1" r="A78" t="n">
+      <c r="D82" t="n">
+        <v>8.0</v>
+      </c>
+      <c s="2" r="E82" t="n">
+        <v>41757.385416666664</v>
+      </c>
+      <c s="2" r="F82" t="n">
+        <v>41757.53125</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6">
+      <c s="1" r="A83" t="n">
         <v>82</v>
       </c>
-      <c s="2" r="B78" t="n">
+      <c s="2" r="B83" t="n">
         <v>41757.385416666664</v>
       </c>
-      <c s="2" r="C78" t="n">
+      <c s="2" r="C83" t="n">
         <v>41757.53125</v>
       </c>
-    </row>
-    <row r="79" spans="1:3">
-      <c s="1" r="A79" t="n">
+      <c r="D83" t="n">
+        <v>3.5</v>
+      </c>
+      <c s="2" r="E83" t="n">
+        <v>41757.885416666664</v>
+      </c>
+      <c s="2" r="F83" t="n">
+        <v>41758.541666666664</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6">
+      <c s="1" r="A84" t="n">
         <v>83</v>
       </c>
-      <c s="2" r="B79" t="n">
+      <c s="2" r="B84" t="n">
         <v>41757.885416666664</v>
       </c>
-      <c s="2" r="C79" t="n">
+      <c s="2" r="C84" t="n">
         <v>41758.541666666664</v>
       </c>
-    </row>
-    <row r="80" spans="1:3">
-      <c s="1" r="A80" t="n">
+      <c r="D84" t="n">
+        <v>15.75</v>
+      </c>
+      <c s="2" r="E84" t="n">
+        <v>41759.489583333336</v>
+      </c>
+      <c s="2" r="F84" t="n">
+        <v>41760.145833333336</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6">
+      <c s="1" r="A85" t="n">
         <v>84</v>
       </c>
-      <c s="2" r="B80" t="n">
+      <c s="2" r="B85" t="n">
         <v>41759.489583333336</v>
       </c>
-      <c s="2" r="C80" t="n">
+      <c s="2" r="C85" t="n">
         <v>41760.145833333336</v>
       </c>
-    </row>
-    <row r="81" spans="1:3">
-      <c s="1" r="A81" t="n">
+      <c r="D85" t="n">
+        <v>15.75</v>
+      </c>
+      <c s="2" r="E85" t="n">
+        <v>41778.5625</v>
+      </c>
+      <c s="2" r="F85" t="n">
+        <v>41778.677083333336</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6">
+      <c s="1" r="A86" t="n">
         <v>85</v>
       </c>
-      <c s="2" r="B81" t="n">
+      <c s="2" r="B86" t="n">
         <v>41778.5625</v>
       </c>
-      <c s="2" r="C81" t="n">
+      <c s="2" r="C86" t="n">
         <v>41778.677083333336</v>
       </c>
-    </row>
-    <row r="82" spans="1:3">
-      <c s="1" r="A82" t="n">
+      <c r="D86" t="n">
+        <v>2.75</v>
+      </c>
+      <c s="2" r="E86" t="n">
+        <v>41779.041666666664</v>
+      </c>
+      <c s="2" r="F86" t="n">
+        <v>41779.1875</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6">
+      <c s="1" r="A87" t="n">
         <v>86</v>
       </c>
-      <c s="2" r="B82" t="n">
+      <c s="2" r="B87" t="n">
         <v>41779.041666666664</v>
       </c>
-      <c s="2" r="C82" t="n">
+      <c s="2" r="C87" t="n">
         <v>41779.1875</v>
       </c>
-    </row>
-    <row r="83" spans="1:3">
-      <c s="1" r="A83" t="n">
+      <c r="D87" t="n">
+        <v>3.5</v>
+      </c>
+      <c s="2" r="E87" t="n">
+        <v>41781.5625</v>
+      </c>
+      <c s="2" r="F87" t="n">
+        <v>41782.104166666664</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6">
+      <c s="1" r="A88" t="n">
         <v>87</v>
       </c>
-      <c s="2" r="B83" t="n">
+      <c s="2" r="B88" t="n">
         <v>41781.5625</v>
       </c>
-      <c s="2" r="C83" t="n">
+      <c s="2" r="C88" t="n">
         <v>41782.104166666664</v>
       </c>
-    </row>
-    <row r="84" spans="1:3">
-      <c s="1" r="A84" t="n">
+      <c r="D88" t="n">
+        <v>13.0</v>
+      </c>
+      <c s="2" r="E88" t="n">
+        <v>41795.802083333336</v>
+      </c>
+      <c s="2" r="F88" t="n">
+        <v>41796.583333333336</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6">
+      <c s="1" r="A89" t="n">
         <v>88</v>
       </c>
-      <c s="2" r="B84" t="n">
+      <c s="2" r="B89" t="n">
         <v>41795.802083333336</v>
       </c>
-      <c s="2" r="C84" t="n">
+      <c s="2" r="C89" t="n">
         <v>41796.583333333336</v>
       </c>
-    </row>
-    <row r="85" spans="1:3">
-      <c s="1" r="A85" t="n">
+      <c r="D89" t="n">
+        <v>18.75</v>
+      </c>
+      <c s="2" r="E89" t="n">
+        <v>41807.072916666664</v>
+      </c>
+      <c s="2" r="F89" t="n">
+        <v>41807.34375</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6">
+      <c s="1" r="A90" t="n">
         <v>89</v>
       </c>
-      <c s="2" r="B85" t="n">
+      <c s="2" r="B90" t="n">
         <v>41807.072916666664</v>
       </c>
-      <c s="2" r="C85" t="n">
+      <c s="2" r="C90" t="n">
         <v>41807.34375</v>
       </c>
-    </row>
-    <row r="86" spans="1:3">
-      <c s="1" r="A86" t="n">
+      <c r="D90" t="n">
+        <v>6.5</v>
+      </c>
+      <c s="2" r="E90" t="n">
+        <v>41823.4375</v>
+      </c>
+      <c s="2" r="F90" t="n">
+        <v>41823.8125</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6">
+      <c s="1" r="A91" t="n">
         <v>90</v>
       </c>
-      <c s="2" r="B86" t="n">
+      <c s="2" r="B91" t="n">
         <v>41823.4375</v>
       </c>
-      <c s="2" r="C86" t="n">
+      <c s="2" r="C91" t="n">
         <v>41823.8125</v>
       </c>
-    </row>
-    <row r="87" spans="1:3">
-      <c s="1" r="A87" t="n">
+      <c r="D91" t="n">
+        <v>9.0</v>
+      </c>
+      <c s="2" r="E91" t="n">
+        <v>41825.25</v>
+      </c>
+      <c s="2" r="F91" t="n">
+        <v>41825.71875</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6">
+      <c s="1" r="A92" t="n">
         <v>91</v>
       </c>
-      <c s="2" r="B87" t="n">
+      <c s="2" r="B92" t="n">
         <v>41825.25</v>
       </c>
-      <c s="2" r="C87" t="n">
+      <c s="2" r="C92" t="n">
         <v>41825.71875</v>
       </c>
-    </row>
-    <row r="88" spans="1:3">
-      <c s="1" r="A88" t="n">
+      <c r="D92" t="n">
+        <v>11.25</v>
+      </c>
+      <c s="2" r="E92" t="n">
+        <v>41826.84375</v>
+      </c>
+      <c s="2" r="F92" t="n">
+        <v>41826.96875</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6">
+      <c s="1" r="A93" t="n">
         <v>92</v>
       </c>
-      <c s="2" r="B88" t="n">
+      <c s="2" r="B93" t="n">
         <v>41826.84375</v>
       </c>
-      <c s="2" r="C88" t="n">
+      <c s="2" r="C93" t="n">
         <v>41826.96875</v>
       </c>
-    </row>
-    <row r="89" spans="1:3">
-      <c s="1" r="A89" t="n">
+      <c r="D93" t="n">
+        <v>3.0</v>
+      </c>
+      <c s="2" r="E93" t="n">
+        <v>41849.25</v>
+      </c>
+      <c s="2" r="F93" t="n">
+        <v>41853.125</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6">
+      <c s="1" r="A94" t="n">
         <v>93</v>
       </c>
-      <c s="2" r="B89" t="n">
+      <c s="2" r="B94" t="n">
         <v>41849.25</v>
       </c>
-      <c s="2" r="C89" t="n">
+      <c s="2" r="C94" t="n">
         <v>41853.125</v>
       </c>
-    </row>
-    <row r="90" spans="1:3">
-      <c s="1" r="A90" t="n">
+      <c r="D94" t="n">
+        <v>93.0</v>
+      </c>
+      <c s="2" r="E94" t="n">
+        <v>41853.552083333336</v>
+      </c>
+      <c s="2" r="F94" t="n">
+        <v>41854.510416666664</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6">
+      <c s="1" r="A95" t="n">
         <v>94</v>
       </c>
-      <c s="2" r="B90" t="n">
+      <c s="2" r="B95" t="n">
         <v>41853.552083333336</v>
       </c>
-      <c s="2" r="C90" t="n">
+      <c s="2" r="C95" t="n">
         <v>41854.510416666664</v>
       </c>
-    </row>
-    <row r="91" spans="1:3">
-      <c s="1" r="A91" t="n">
+      <c r="D95" t="n">
+        <v>23.0</v>
+      </c>
+      <c s="2" r="E95" t="n">
+        <v>41927.53125</v>
+      </c>
+      <c s="2" r="F95" t="n">
+        <v>41927.697916666664</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6">
+      <c s="1" r="A96" t="n">
         <v>95</v>
       </c>
-      <c s="2" r="B91" t="n">
+      <c s="2" r="B96" t="n">
         <v>41927.53125</v>
       </c>
-      <c s="2" r="C91" t="n">
+      <c s="2" r="C96" t="n">
         <v>41927.697916666664</v>
       </c>
-    </row>
-    <row r="92" spans="1:3">
-      <c s="1" r="A92" t="n">
+      <c r="D96" t="n">
+        <v>4.0</v>
+      </c>
+      <c s="2" r="E96" t="n">
+        <v>41927.739583333336</v>
+      </c>
+      <c s="2" r="F96" t="n">
+        <v>41928.114583333336</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6">
+      <c s="1" r="A97" t="n">
         <v>96</v>
       </c>
-      <c s="2" r="B92" t="n">
+      <c s="2" r="B97" t="n">
         <v>41927.739583333336</v>
       </c>
-      <c s="2" r="C92" t="n">
+      <c s="2" r="C97" t="n">
         <v>41928.114583333336</v>
       </c>
-    </row>
-    <row r="93" spans="1:3">
-      <c s="1" r="A93" t="n">
+      <c r="D97" t="n">
+        <v>9.0</v>
+      </c>
+      <c s="2" r="E97" t="n">
+        <v>41945.072916666664</v>
+      </c>
+      <c s="2" r="F97" t="n">
+        <v>41945.385416666664</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6">
+      <c s="1" r="A98" t="n">
         <v>97</v>
       </c>
-      <c s="2" r="B93" t="n">
+      <c s="2" r="B98" t="n">
         <v>41945.072916666664</v>
       </c>
-      <c s="2" r="C93" t="n">
+      <c s="2" r="C98" t="n">
         <v>41945.385416666664</v>
+      </c>
+      <c r="D98" t="n">
+        <v>7.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>